<commit_message>
Nuovo test con testata jwt corretta
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111#JOKERSRLXX/JOKER SRL/MGCup/1.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111#JOKERSRLXX/JOKER SRL/MGCup/1.0/report-checklist.xlsx
@@ -1320,16 +1320,16 @@
 </t>
   </si>
   <si>
-    <t>28/11/2024</t>
-  </si>
-  <si>
-    <t>2024-11-28T17:49:48Z</t>
-  </si>
-  <si>
-    <t>2adcf6690a8ba804</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.57d34093d4^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>06/12/2024</t>
+  </si>
+  <si>
+    <t>2024-12-06T11:28:24Z</t>
+  </si>
+  <si>
+    <t>6b3b63f66dac6a01</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.a3bd832750^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RSA_CT2</t>
@@ -1340,13 +1340,13 @@
 </t>
   </si>
   <si>
-    <t>2024-11-28T17:00:51Z</t>
-  </si>
-  <si>
-    <t>b5438fd6e2caee32</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.8b99257462^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2024-12-06T11:29:38Z</t>
+  </si>
+  <si>
+    <t>294470ec8cf93ffd</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.ebe968306f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RSA_CT3</t>
@@ -1357,13 +1357,13 @@
 </t>
   </si>
   <si>
-    <t>2024-11-28T17:06:41Z</t>
-  </si>
-  <si>
-    <t>c3a5dd0ef2559fa4</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.3d9793c45e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2024-12-06T11:30:30Z</t>
+  </si>
+  <si>
+    <t>70a9f63dbe812ca2</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.ab9b260ab1^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RSA_CT4</t>
@@ -1374,13 +1374,13 @@
 </t>
   </si>
   <si>
-    <t>2024-11-28T17:47:25Z</t>
-  </si>
-  <si>
-    <t>0b418e2a605b362f</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.e5aa030296^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2024-12-06T11:31:21Z</t>
+  </si>
+  <si>
+    <t>22cb3bfc46af90b4</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.69010c1bfc^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RSA_CT5_KO</t>
@@ -1699,13 +1699,13 @@
 </t>
   </si>
   <si>
-    <t>2024-11-28T17:52:06Z</t>
-  </si>
-  <si>
-    <t>354fa05348926c79</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.17b7492821^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2024-12-06T11:32:13Z</t>
+  </si>
+  <si>
+    <t>5b321e0dc85892d5</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.cdb0bb1b74^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_LAB_TRASF_CT2</t>

</xml_diff>